<commit_message>
Commiting execution branch to main
</commit_message>
<xml_diff>
--- a/SwagLabDataProvider/src/main/java/com/testData/MyTestData07May.xlsx
+++ b/SwagLabDataProvider/src/main/java/com/testData/MyTestData07May.xlsx
@@ -13,7 +13,7 @@
   <calcPr calcId="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>usernames </t>
   </si>
@@ -42,12 +42,16 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,8 +438,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.5546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.88671875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -452,6 +456,9 @@
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">

</xml_diff>